<commit_message>
updating the variable descriptions Excel file
</commit_message>
<xml_diff>
--- a/Task1_KFC-team-coding/data/KFC-team_pizza-variables.xlsx
+++ b/Task1_KFC-team-coding/data/KFC-team_pizza-variables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/sule_kata_student_ceu_edu/Documents/DA-1_KFC-team_Team-Assignment-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEU\Fall_Term\Github_Repos\homework_codesANDmore_Coding1_MScBA\Task1_KFC-team-coding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CC2F2B6-4A4B-46ED-A353-97FBF0EFD636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0762C4-67BE-406A-A0FD-33DE4BC0EBC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Variable</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Data Type on Computer</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>Address of the restaurant, contains house number and street name.</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Qualitative, binary</t>
   </si>
   <si>
-    <t>Logical</t>
-  </si>
-  <si>
     <t>The variable shows whether the prices (price_pizza and price_swater) are for an on-site restaurant or delivery to CEU Budapest Campus (1051 Budapest, Nádor Street 15.). Possible values are: Yes (delivery), No (on-site).</t>
   </si>
   <si>
@@ -163,13 +154,19 @@
   </si>
   <si>
     <t>Wolt</t>
+  </si>
+  <si>
+    <t>Data Type in R</t>
+  </si>
+  <si>
+    <t>Character</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -549,17 +546,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="216.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="216.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,236 +564,236 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="3">
         <v>1300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
       </c>
       <c r="F6" s="3">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E8" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>